<commit_message>
added concrete pad layout
</commit_message>
<xml_diff>
--- a/HCRO-Power-Distribution/Heat-Load-Calculation.xlsx
+++ b/HCRO-Power-Distribution/Heat-Load-Calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/HVAC-Signal-Processing-Room/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/HCRO-Power-Distribution/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44871A1E-9042-8E4A-9729-1BC5703A3301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B4E466-57DC-F343-B221-54B32709BBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5440" yWindow="460" windowWidth="24580" windowHeight="19700" xr2:uid="{D45A1780-0C9F-B74A-8B8A-CFC9344D9ADA}"/>
+    <workbookView xWindow="5440" yWindow="780" windowWidth="24580" windowHeight="19700" xr2:uid="{D45A1780-0C9F-B74A-8B8A-CFC9344D9ADA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -220,24 +220,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -246,7 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -267,9 +259,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +299,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -413,7 +405,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -555,7 +547,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -565,61 +557,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06675C7E-7244-CA47-BE3B-A2B799861F4B}">
   <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="13"/>
       <c r="F4">
         <v>20</v>
       </c>
@@ -633,19 +611,12 @@
       <c r="I4" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16"/>
+      <c r="B5" s="13"/>
       <c r="F5">
         <v>4</v>
       </c>
@@ -659,19 +630,12 @@
       <c r="I5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="16"/>
+      <c r="B6" s="13"/>
       <c r="F6">
         <v>4</v>
       </c>
@@ -685,22 +649,6 @@
       <c r="I6" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
     </row>
     <row r="8" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="H8" s="3">
@@ -710,67 +658,43 @@
       <c r="I8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="10"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
-      <c r="O10" s="10"/>
-      <c r="P10" s="10"/>
-    </row>
+    </row>
+    <row r="9" spans="1:16" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="20"/>
+      <c r="A12" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="12"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="13"/>
       <c r="D14">
         <v>1</v>
       </c>
@@ -792,10 +716,10 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="13"/>
       <c r="D15">
         <v>1</v>
       </c>
@@ -817,10 +741,10 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="14"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1">
         <v>1</v>
@@ -843,10 +767,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="13"/>
       <c r="D17">
         <v>1</v>
       </c>
@@ -868,10 +792,10 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="16"/>
+      <c r="B18" s="13"/>
       <c r="D18">
         <v>6</v>
       </c>
@@ -893,10 +817,10 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="16"/>
+      <c r="B19" s="13"/>
       <c r="D19">
         <v>8</v>
       </c>
@@ -918,10 +842,10 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="16"/>
+      <c r="B20" s="13"/>
       <c r="D20">
         <v>1</v>
       </c>
@@ -943,10 +867,10 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="16"/>
+      <c r="B21" s="13"/>
       <c r="D21">
         <v>1</v>
       </c>
@@ -968,10 +892,10 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="16"/>
+      <c r="B22" s="13"/>
       <c r="D22">
         <v>2</v>
       </c>
@@ -993,10 +917,10 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="16"/>
+      <c r="B23" s="13"/>
       <c r="D23">
         <v>1</v>
       </c>
@@ -1018,10 +942,10 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="16"/>
+      <c r="B24" s="13"/>
       <c r="D24">
         <v>4</v>
       </c>
@@ -1043,10 +967,10 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="18"/>
+      <c r="B25" s="14"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1">
         <v>1</v>
@@ -1069,10 +993,10 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="16" t="s">
+      <c r="A26" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="16"/>
+      <c r="B26" s="13"/>
       <c r="D26">
         <v>12</v>
       </c>
@@ -1094,10 +1018,10 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="16" t="s">
+      <c r="A27" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="16"/>
+      <c r="B27" s="13"/>
       <c r="D27">
         <v>5</v>
       </c>
@@ -1119,46 +1043,45 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14">
+      <c r="B28" s="13"/>
+      <c r="D28">
         <v>5</v>
       </c>
-      <c r="E28" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F28" s="14">
+      <c r="E28" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28">
         <v>100</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="H28" s="14">
+      <c r="G28" t="s">
+        <v>10</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H30" s="7">
+      <c r="H30" s="6">
         <f>SUM(H14:H28)</f>
         <v>25.650000000000002</v>
       </c>
-      <c r="I30" s="8" t="s">
+      <c r="I30" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H31" s="12">
+      <c r="H31" s="10">
         <f>$H$8-H30</f>
         <v>72.82186999999999</v>
       </c>
-      <c r="I31" s="13" t="s">
+      <c r="I31" s="11" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1171,33 +1094,33 @@
       <c r="B33" s="5"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="20"/>
+      <c r="A35" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="12"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="16"/>
+      <c r="B37" s="13"/>
       <c r="D37">
         <v>1</v>
       </c>
@@ -1219,10 +1142,10 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="16" t="s">
+      <c r="A38" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="16"/>
+      <c r="B38" s="13"/>
       <c r="D38">
         <v>1</v>
       </c>
@@ -1244,10 +1167,10 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="18"/>
+      <c r="B39" s="14"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1">
         <v>1</v>
@@ -1270,10 +1193,10 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="16"/>
+      <c r="B40" s="13"/>
       <c r="D40">
         <v>1</v>
       </c>
@@ -1295,10 +1218,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B41" s="16"/>
+      <c r="B41" s="13"/>
       <c r="D41">
         <v>6</v>
       </c>
@@ -1320,36 +1243,36 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11">
+      <c r="B42" s="16"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9">
         <v>43</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" s="11">
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="9">
         <v>1300</v>
       </c>
-      <c r="G42" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H42" s="11">
+      <c r="G42" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H42" s="9">
         <f t="shared" si="2"/>
         <v>55.9</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I42" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B43" s="16"/>
+      <c r="B43" s="13"/>
       <c r="D43">
         <v>1</v>
       </c>
@@ -1371,10 +1294,10 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B44" s="16"/>
+      <c r="B44" s="13"/>
       <c r="D44">
         <v>1</v>
       </c>
@@ -1396,10 +1319,10 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="16"/>
+      <c r="B45" s="13"/>
       <c r="D45">
         <v>2</v>
       </c>
@@ -1421,10 +1344,10 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B46" s="16"/>
+      <c r="B46" s="13"/>
       <c r="D46">
         <v>1</v>
       </c>
@@ -1446,10 +1369,10 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B47" s="16"/>
+      <c r="B47" s="13"/>
       <c r="D47">
         <v>4</v>
       </c>
@@ -1471,10 +1394,10 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B48" s="18"/>
+      <c r="B48" s="14"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1">
         <v>1</v>
@@ -1497,10 +1420,10 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B49" s="16"/>
+      <c r="B49" s="13"/>
       <c r="D49">
         <v>12</v>
       </c>
@@ -1522,54 +1445,54 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11">
+      <c r="B50" s="16"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9">
         <v>22</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F50" s="11">
+      <c r="E50" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="9">
         <v>50</v>
       </c>
-      <c r="G50" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H50" s="11">
+      <c r="G50" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H50" s="9">
         <f t="shared" si="2"/>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I50" s="11" t="s">
+      <c r="I50" s="9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="17"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11">
+      <c r="B51" s="16"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9">
         <v>21</v>
       </c>
-      <c r="E51" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="F51" s="11">
+      <c r="E51" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" s="9">
         <v>180</v>
       </c>
-      <c r="G51" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="11">
+      <c r="G51" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="9">
         <f t="shared" si="2"/>
         <v>3.78</v>
       </c>
-      <c r="I51" s="11" t="s">
+      <c r="I51" s="9" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1578,33 +1501,40 @@
       <c r="B52" s="5"/>
     </row>
     <row r="54" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="H54" s="7">
+      <c r="H54" s="6">
         <f>SUM(H37:H51)</f>
         <v>75.279999999999987</v>
       </c>
-      <c r="I54" s="8" t="s">
+      <c r="I54" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="H55" s="12">
+      <c r="H55" s="10">
         <f>$H$8-H54</f>
         <v>23.191870000000009</v>
       </c>
-      <c r="I55" s="13" t="s">
+      <c r="I55" s="11" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A1:I1"/>
@@ -1621,21 +1551,14 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>